<commit_message>
OCT 25 update, removed phone number
</commit_message>
<xml_diff>
--- a/data/collaborations.xlsx
+++ b/data/collaborations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conorisco/Dropbox (Personal)/Jobs/CV and Publications/CV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4846C781-B495-B44B-B47E-68B1CDEF0378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF685B4-E6EA-1A4F-B2E6-13E37AA01934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="760" windowWidth="17280" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="1960" windowWidth="27960" windowHeight="22740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>what</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Lara Dungan, Niall Conlon</t>
   </si>
   <si>
-    <t>Information withheld</t>
-  </si>
-  <si>
     <t xml:space="preserve">Title withheld, microglia focused (mouse) </t>
   </si>
   <si>
@@ -222,16 +219,52 @@
     <t>Study design, bioinformatics, training, scientific input</t>
   </si>
   <si>
-    <t>Title withheld</t>
-  </si>
-  <si>
     <t>The pleural cavity macrophage proteome</t>
   </si>
   <si>
     <t>Role of CD40 signalling in tissue resident macrophage proliferation</t>
   </si>
   <si>
-    <t>Legend Biotech &amp; Tony McElligott</t>
+    <t>Legend Biotech, Tony Mc Elligott &amp; Nina Orfali</t>
+  </si>
+  <si>
+    <t>Blood Cancer, Title withheld</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>Title withheald</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Luara Gleeson</t>
+  </si>
+  <si>
+    <t>2024-Present</t>
+  </si>
+  <si>
+    <t>Human Pleural biology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kathy Gately </t>
+  </si>
+  <si>
+    <t>2025-Present</t>
+  </si>
+  <si>
+    <t>TCD, St James' Hospital</t>
+  </si>
+  <si>
+    <t>Malignang Pleural Effussion</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -627,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -642,7 +675,7 @@
     <col min="5" max="5" width="117.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -658,8 +691,11 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -676,7 +712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -690,24 +726,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -723,8 +762,11 @@
       <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
@@ -740,8 +782,11 @@
       <c r="E6" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
@@ -757,13 +802,16 @@
       <c r="E7" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F7" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>26</v>
@@ -774,8 +822,11 @@
       <c r="E8" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="F8" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
@@ -791,8 +842,11 @@
       <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="F9" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -808,8 +862,11 @@
       <c r="E10" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F10" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -823,10 +880,13 @@
         <v>22</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
@@ -840,10 +900,13 @@
         <v>8</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -859,8 +922,11 @@
       <c r="E13" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F13" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>41</v>
       </c>
@@ -876,8 +942,11 @@
       <c r="E14" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F14" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>47</v>
       </c>
@@ -893,8 +962,11 @@
       <c r="E15" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F15" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
@@ -908,10 +980,13 @@
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>49</v>
       </c>
@@ -925,24 +1000,64 @@
         <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>